<commit_message>
feature: Ajustado para variavel a linha final da planilha, correções
</commit_message>
<xml_diff>
--- a/planilhas/Rel_atividades 08-2024 KevinSilva.xlsx
+++ b/planilhas/Rel_atividades 08-2024 KevinSilva.xlsx
@@ -857,10 +857,10 @@
       <c r="C10" s="26" t="n"/>
       <c r="D10" s="37" t="n"/>
       <c r="E10" s="59" t="n">
-        <v>0.33125</v>
+        <v>0.3326388888888889</v>
       </c>
       <c r="F10" s="59" t="n">
-        <v>0.5020833333333333</v>
+        <v>0.4993055555555556</v>
       </c>
       <c r="G10" s="16">
         <f>F10-E10</f>
@@ -877,10 +877,10 @@
       <c r="C11" s="13" t="n"/>
       <c r="D11" s="38" t="n"/>
       <c r="E11" s="60" t="n">
-        <v>0.5826388888888889</v>
+        <v>0.5847222222222223</v>
       </c>
       <c r="F11" s="60" t="n">
-        <v>0.7527777777777778</v>
+        <v>0.7597222222222222</v>
       </c>
       <c r="G11" s="21">
         <f>F11-E11</f>
@@ -902,10 +902,10 @@
       <c r="C12" s="26" t="n"/>
       <c r="D12" s="37" t="n"/>
       <c r="E12" s="59" t="n">
-        <v>0.3368055555555556</v>
+        <v>0.3354166666666666</v>
       </c>
       <c r="F12" s="59" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.5</v>
       </c>
       <c r="G12" s="16">
         <f>F12-E12</f>
@@ -922,10 +922,10 @@
       <c r="C13" s="13" t="n"/>
       <c r="D13" s="38" t="n"/>
       <c r="E13" s="60" t="n">
-        <v>0.5888888888888889</v>
+        <v>0.5854166666666667</v>
       </c>
       <c r="F13" s="60" t="n">
-        <v>0.7513888888888889</v>
+        <v>0.7472222222222222</v>
       </c>
       <c r="G13" s="21">
         <f>F13-E13</f>
@@ -951,10 +951,10 @@
       <c r="C14" s="23" t="n"/>
       <c r="D14" s="23" t="n"/>
       <c r="E14" s="61" t="n">
-        <v>0.3340277777777778</v>
+        <v>0.3305555555555555</v>
       </c>
       <c r="F14" s="61" t="n">
-        <v>0.5027777777777778</v>
+        <v>0.5020833333333333</v>
       </c>
       <c r="G14" s="19" t="n"/>
       <c r="H14" s="34" t="n"/>
@@ -972,10 +972,10 @@
       <c r="C15" s="23" t="n"/>
       <c r="D15" s="23" t="n"/>
       <c r="E15" s="61" t="n">
-        <v>0.5875</v>
+        <v>0.5798611111111112</v>
       </c>
       <c r="F15" s="61" t="n">
-        <v>0.7590277777777777</v>
+        <v>0.7506944444444444</v>
       </c>
       <c r="G15" s="19" t="n"/>
       <c r="H15" s="34" t="n"/>
@@ -989,10 +989,10 @@
       <c r="C16" s="26" t="n"/>
       <c r="D16" s="37" t="n"/>
       <c r="E16" s="59" t="n">
-        <v>0.3347222222222222</v>
+        <v>0.3340277777777778</v>
       </c>
       <c r="F16" s="59" t="n">
-        <v>0.5027777777777778</v>
+        <v>0.4979166666666667</v>
       </c>
       <c r="G16" s="16">
         <f>F16-E16</f>
@@ -1009,7 +1009,7 @@
       <c r="C17" s="13" t="n"/>
       <c r="D17" s="38" t="n"/>
       <c r="E17" s="60" t="n">
-        <v>0.5819444444444445</v>
+        <v>0.5888888888888889</v>
       </c>
       <c r="F17" s="60" t="n">
         <v>0.7486111111111111</v>
@@ -1034,10 +1034,10 @@
       <c r="C18" s="26" t="n"/>
       <c r="D18" s="37" t="n"/>
       <c r="E18" s="59" t="n">
-        <v>0.3368055555555556</v>
+        <v>0.3347222222222222</v>
       </c>
       <c r="F18" s="59" t="n">
-        <v>0.4972222222222222</v>
+        <v>0.5027777777777778</v>
       </c>
       <c r="G18" s="16">
         <f>F18-E18</f>
@@ -1054,10 +1054,10 @@
       <c r="C19" s="13" t="n"/>
       <c r="D19" s="38" t="n"/>
       <c r="E19" s="60" t="n">
-        <v>0.5923611111111111</v>
+        <v>0.58125</v>
       </c>
       <c r="F19" s="60" t="n">
-        <v>0.7465277777777778</v>
+        <v>0.7513888888888889</v>
       </c>
       <c r="G19" s="21">
         <f>F19-E19</f>
@@ -1079,10 +1079,10 @@
       <c r="C20" s="26" t="n"/>
       <c r="D20" s="37" t="n"/>
       <c r="E20" s="59" t="n">
-        <v>0.3340277777777778</v>
+        <v>0.33125</v>
       </c>
       <c r="F20" s="59" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.4993055555555556</v>
       </c>
       <c r="G20" s="16">
         <f>F20-E20</f>
@@ -1099,10 +1099,10 @@
       <c r="C21" s="13" t="n"/>
       <c r="D21" s="38" t="n"/>
       <c r="E21" s="60" t="n">
-        <v>0.5909722222222222</v>
+        <v>0.58125</v>
       </c>
       <c r="F21" s="60" t="n">
-        <v>0.7527777777777778</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="G21" s="21">
         <f>F21-E21</f>
@@ -1124,10 +1124,10 @@
       <c r="C22" s="26" t="n"/>
       <c r="D22" s="37" t="n"/>
       <c r="E22" s="59" t="n">
-        <v>0.3340277777777778</v>
+        <v>0.3347222222222222</v>
       </c>
       <c r="F22" s="59" t="n">
-        <v>0.4993055555555556</v>
+        <v>0.5006944444444444</v>
       </c>
       <c r="G22" s="16">
         <f>F22-E22</f>
@@ -1144,10 +1144,10 @@
       <c r="C23" s="13" t="n"/>
       <c r="D23" s="38" t="n"/>
       <c r="E23" s="60" t="n">
-        <v>0.5875</v>
+        <v>0.5930555555555556</v>
       </c>
       <c r="F23" s="60" t="n">
-        <v>0.7486111111111111</v>
+        <v>0.7506944444444444</v>
       </c>
       <c r="G23" s="21">
         <f>F23-E23</f>
@@ -1169,10 +1169,10 @@
       <c r="C24" s="26" t="n"/>
       <c r="D24" s="37" t="n"/>
       <c r="E24" s="59" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.33125</v>
       </c>
       <c r="F24" s="59" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.4972222222222222</v>
       </c>
       <c r="G24" s="16">
         <f>F24-E24</f>
@@ -1189,10 +1189,10 @@
       <c r="C25" s="13" t="n"/>
       <c r="D25" s="38" t="n"/>
       <c r="E25" s="60" t="n">
-        <v>0.5819444444444445</v>
+        <v>0.5895833333333333</v>
       </c>
       <c r="F25" s="60" t="n">
-        <v>0.7506944444444444</v>
+        <v>0.7493055555555556</v>
       </c>
       <c r="G25" s="21">
         <f>F25-E25</f>
@@ -1218,10 +1218,10 @@
       <c r="C26" s="23" t="n"/>
       <c r="D26" s="23" t="n"/>
       <c r="E26" s="61" t="n">
-        <v>0.3305555555555555</v>
+        <v>0.33125</v>
       </c>
       <c r="F26" s="61" t="n">
-        <v>0.5006944444444444</v>
+        <v>0.5</v>
       </c>
       <c r="G26" s="19" t="n"/>
       <c r="H26" s="34" t="n"/>
@@ -1239,10 +1239,10 @@
       <c r="C27" s="23" t="n"/>
       <c r="D27" s="23" t="n"/>
       <c r="E27" s="61" t="n">
-        <v>0.5916666666666667</v>
+        <v>0.58125</v>
       </c>
       <c r="F27" s="61" t="n">
-        <v>0.7604166666666666</v>
+        <v>0.7569444444444444</v>
       </c>
       <c r="G27" s="19" t="n"/>
       <c r="H27" s="34" t="n"/>
@@ -1256,10 +1256,10 @@
       <c r="C28" s="26" t="n"/>
       <c r="D28" s="37" t="n"/>
       <c r="E28" s="59" t="n">
-        <v>0.3319444444444444</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F28" s="59" t="n">
-        <v>0.4993055555555556</v>
+        <v>0.5013888888888889</v>
       </c>
       <c r="G28" s="16">
         <f>F28-E28</f>
@@ -1276,10 +1276,10 @@
       <c r="C29" s="13" t="n"/>
       <c r="D29" s="38" t="n"/>
       <c r="E29" s="60" t="n">
-        <v>0.5881944444444445</v>
+        <v>0.5798611111111112</v>
       </c>
       <c r="F29" s="60" t="n">
-        <v>0.7534722222222222</v>
+        <v>0.7493055555555556</v>
       </c>
       <c r="G29" s="21">
         <f>F29-E29</f>
@@ -1301,7 +1301,7 @@
       <c r="C30" s="26" t="n"/>
       <c r="D30" s="37" t="n"/>
       <c r="E30" s="59" t="n">
-        <v>0.3319444444444444</v>
+        <v>0.3347222222222222</v>
       </c>
       <c r="F30" s="59" t="n">
         <v>0.5027777777777778</v>
@@ -1321,10 +1321,10 @@
       <c r="C31" s="13" t="n"/>
       <c r="D31" s="38" t="n"/>
       <c r="E31" s="60" t="n">
-        <v>0.5881944444444445</v>
+        <v>0.5798611111111112</v>
       </c>
       <c r="F31" s="60" t="n">
-        <v>0.7472222222222222</v>
+        <v>0.7486111111111111</v>
       </c>
       <c r="G31" s="21">
         <f>F31-E31</f>
@@ -1349,7 +1349,7 @@
         <v>0.3326388888888889</v>
       </c>
       <c r="F32" s="59" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.5027777777777778</v>
       </c>
       <c r="G32" s="16">
         <f>F32-E32</f>
@@ -1366,10 +1366,10 @@
       <c r="C33" s="13" t="n"/>
       <c r="D33" s="38" t="n"/>
       <c r="E33" s="60" t="n">
-        <v>0.58125</v>
+        <v>0.5868055555555556</v>
       </c>
       <c r="F33" s="60" t="n">
-        <v>0.7520833333333333</v>
+        <v>0.7479166666666667</v>
       </c>
       <c r="G33" s="21">
         <f>F33-E33</f>
@@ -1391,10 +1391,10 @@
       <c r="C34" s="26" t="n"/>
       <c r="D34" s="37" t="n"/>
       <c r="E34" s="59" t="n">
-        <v>0.3361111111111111</v>
+        <v>0.3305555555555555</v>
       </c>
       <c r="F34" s="59" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.4986111111111111</v>
       </c>
       <c r="G34" s="16">
         <f>F34-E34</f>
@@ -1411,10 +1411,10 @@
       <c r="C35" s="13" t="n"/>
       <c r="D35" s="38" t="n"/>
       <c r="E35" s="60" t="n">
-        <v>0.5847222222222223</v>
+        <v>0.5819444444444445</v>
       </c>
       <c r="F35" s="60" t="n">
-        <v>0.7493055555555556</v>
+        <v>0.7520833333333333</v>
       </c>
       <c r="G35" s="21">
         <f>F35-E35</f>
@@ -1436,10 +1436,10 @@
       <c r="C36" s="26" t="n"/>
       <c r="D36" s="37" t="n"/>
       <c r="E36" s="59" t="n">
-        <v>0.3326388888888889</v>
+        <v>0.3319444444444444</v>
       </c>
       <c r="F36" s="59" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.5027777777777778</v>
       </c>
       <c r="G36" s="16">
         <f>F36-E36</f>
@@ -1456,10 +1456,10 @@
       <c r="C37" s="13" t="n"/>
       <c r="D37" s="38" t="n"/>
       <c r="E37" s="60" t="n">
-        <v>0.5861111111111111</v>
+        <v>0.5881944444444445</v>
       </c>
       <c r="F37" s="60" t="n">
-        <v>0.7527777777777778</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="G37" s="21">
         <f>F37-E37</f>
@@ -1488,7 +1488,7 @@
         <v>0.3354166666666666</v>
       </c>
       <c r="F38" s="61" t="n">
-        <v>0.4986111111111111</v>
+        <v>0.5006944444444444</v>
       </c>
       <c r="G38" s="19" t="n"/>
       <c r="H38" s="34" t="n"/>
@@ -1509,7 +1509,7 @@
         <v>0.5798611111111112</v>
       </c>
       <c r="F39" s="61" t="n">
-        <v>0.7479166666666667</v>
+        <v>0.7472222222222222</v>
       </c>
       <c r="G39" s="19" t="n"/>
       <c r="H39" s="34" t="n"/>
@@ -1523,10 +1523,10 @@
       <c r="C40" s="26" t="n"/>
       <c r="D40" s="37" t="n"/>
       <c r="E40" s="59" t="n">
-        <v>0.33125</v>
+        <v>0.3368055555555556</v>
       </c>
       <c r="F40" s="59" t="n">
-        <v>0.4993055555555556</v>
+        <v>0.5034722222222222</v>
       </c>
       <c r="G40" s="16">
         <f>F40-E40</f>
@@ -1546,7 +1546,7 @@
         <v>0.5854166666666667</v>
       </c>
       <c r="F41" s="60" t="n">
-        <v>0.75625</v>
+        <v>0.7479166666666667</v>
       </c>
       <c r="G41" s="21">
         <f>F41-E41</f>
@@ -1568,10 +1568,10 @@
       <c r="C42" s="26" t="n"/>
       <c r="D42" s="37" t="n"/>
       <c r="E42" s="59" t="n">
-        <v>0.3347222222222222</v>
+        <v>0.3340277777777778</v>
       </c>
       <c r="F42" s="59" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.4993055555555556</v>
       </c>
       <c r="G42" s="16">
         <f>F42-E42</f>
@@ -1588,10 +1588,10 @@
       <c r="C43" s="13" t="n"/>
       <c r="D43" s="38" t="n"/>
       <c r="E43" s="60" t="n">
-        <v>0.5930555555555556</v>
+        <v>0.5909722222222222</v>
       </c>
       <c r="F43" s="60" t="n">
-        <v>0.7472222222222222</v>
+        <v>0.7576388888888889</v>
       </c>
       <c r="G43" s="21">
         <f>F43-E43</f>
@@ -1613,10 +1613,10 @@
       <c r="C44" s="26" t="n"/>
       <c r="D44" s="37" t="n"/>
       <c r="E44" s="59" t="n">
-        <v>0.3340277777777778</v>
+        <v>0.3319444444444444</v>
       </c>
       <c r="F44" s="59" t="n">
-        <v>0.5013888888888889</v>
+        <v>0.4993055555555556</v>
       </c>
       <c r="G44" s="16">
         <f>F44-E44</f>
@@ -1633,10 +1633,10 @@
       <c r="C45" s="13" t="n"/>
       <c r="D45" s="38" t="n"/>
       <c r="E45" s="60" t="n">
-        <v>0.5833333333333334</v>
+        <v>0.5881944444444445</v>
       </c>
       <c r="F45" s="60" t="n">
-        <v>0.7597222222222222</v>
+        <v>0.7520833333333333</v>
       </c>
       <c r="G45" s="21">
         <f>F45-E45</f>
@@ -1658,10 +1658,10 @@
       <c r="C46" s="26" t="n"/>
       <c r="D46" s="37" t="n"/>
       <c r="E46" s="59" t="n">
-        <v>0.3361111111111111</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F46" s="59" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.5027777777777778</v>
       </c>
       <c r="G46" s="16">
         <f>F46-E46</f>
@@ -1678,10 +1678,10 @@
       <c r="C47" s="13" t="n"/>
       <c r="D47" s="38" t="n"/>
       <c r="E47" s="60" t="n">
-        <v>0.5895833333333333</v>
+        <v>0.5798611111111112</v>
       </c>
       <c r="F47" s="60" t="n">
-        <v>0.7472222222222222</v>
+        <v>0.7534722222222222</v>
       </c>
       <c r="G47" s="21">
         <f>F47-E47</f>
@@ -1703,10 +1703,10 @@
       <c r="C48" s="26" t="n"/>
       <c r="D48" s="37" t="n"/>
       <c r="E48" s="59" t="n">
-        <v>0.3340277777777778</v>
+        <v>0.33125</v>
       </c>
       <c r="F48" s="59" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.4972222222222222</v>
       </c>
       <c r="G48" s="16">
         <f>F48-E48</f>
@@ -1723,10 +1723,10 @@
       <c r="C49" s="13" t="n"/>
       <c r="D49" s="38" t="n"/>
       <c r="E49" s="60" t="n">
-        <v>0.5819444444444445</v>
+        <v>0.5868055555555556</v>
       </c>
       <c r="F49" s="60" t="n">
-        <v>0.7493055555555556</v>
+        <v>0.7479166666666667</v>
       </c>
       <c r="G49" s="21">
         <f>F49-E49</f>
@@ -1752,10 +1752,10 @@
       <c r="C50" s="23" t="n"/>
       <c r="D50" s="23" t="n"/>
       <c r="E50" s="61" t="n">
-        <v>0.3361111111111111</v>
+        <v>0.3354166666666666</v>
       </c>
       <c r="F50" s="61" t="n">
-        <v>0.4972222222222222</v>
+        <v>0.5020833333333333</v>
       </c>
       <c r="G50" s="19" t="n"/>
       <c r="H50" s="34" t="n"/>
@@ -1773,10 +1773,10 @@
       <c r="C51" s="23" t="n"/>
       <c r="D51" s="23" t="n"/>
       <c r="E51" s="61" t="n">
-        <v>0.5902777777777778</v>
+        <v>0.5805555555555556</v>
       </c>
       <c r="F51" s="61" t="n">
-        <v>0.7472222222222222</v>
+        <v>0.7486111111111111</v>
       </c>
       <c r="G51" s="19" t="n"/>
       <c r="H51" s="34" t="n"/>
@@ -1793,7 +1793,7 @@
         <v>0.3319444444444444</v>
       </c>
       <c r="F52" s="59" t="n">
-        <v>0.4972222222222222</v>
+        <v>0.5</v>
       </c>
       <c r="G52" s="16">
         <f>F52-E52</f>
@@ -1810,10 +1810,10 @@
       <c r="C53" s="13" t="n"/>
       <c r="D53" s="38" t="n"/>
       <c r="E53" s="60" t="n">
-        <v>0.5805555555555556</v>
+        <v>0.5868055555555556</v>
       </c>
       <c r="F53" s="60" t="n">
-        <v>0.7472222222222222</v>
+        <v>0.75</v>
       </c>
       <c r="G53" s="21">
         <f>F53-E53</f>
@@ -1835,10 +1835,10 @@
       <c r="C54" s="26" t="n"/>
       <c r="D54" s="37" t="n"/>
       <c r="E54" s="59" t="n">
-        <v>0.3347222222222222</v>
+        <v>0.3319444444444444</v>
       </c>
       <c r="F54" s="59" t="n">
-        <v>0.4979166666666667</v>
+        <v>0.5006944444444444</v>
       </c>
       <c r="G54" s="16">
         <f>F54-E54</f>
@@ -1855,10 +1855,10 @@
       <c r="C55" s="13" t="n"/>
       <c r="D55" s="38" t="n"/>
       <c r="E55" s="60" t="n">
-        <v>0.5798611111111112</v>
+        <v>0.5819444444444445</v>
       </c>
       <c r="F55" s="60" t="n">
-        <v>0.7493055555555556</v>
+        <v>0.75</v>
       </c>
       <c r="G55" s="21">
         <f>F55-E55</f>
@@ -1880,10 +1880,10 @@
       <c r="C56" s="26" t="n"/>
       <c r="D56" s="37" t="n"/>
       <c r="E56" s="59" t="n">
-        <v>0.3347222222222222</v>
+        <v>0.3361111111111111</v>
       </c>
       <c r="F56" s="59" t="n">
-        <v>0.5</v>
+        <v>0.4965277777777778</v>
       </c>
       <c r="G56" s="16">
         <f>F56-E56</f>
@@ -1900,10 +1900,10 @@
       <c r="C57" s="13" t="n"/>
       <c r="D57" s="38" t="n"/>
       <c r="E57" s="60" t="n">
-        <v>0.5826388888888889</v>
+        <v>0.5916666666666667</v>
       </c>
       <c r="F57" s="60" t="n">
-        <v>0.7520833333333333</v>
+        <v>0.7472222222222222</v>
       </c>
       <c r="G57" s="21">
         <f>F57-E57</f>
@@ -1925,10 +1925,10 @@
       <c r="C58" s="26" t="n"/>
       <c r="D58" s="37" t="n"/>
       <c r="E58" s="59" t="n">
-        <v>0.3354166666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F58" s="59" t="n">
-        <v>0.4986111111111111</v>
+        <v>0.5020833333333333</v>
       </c>
       <c r="G58" s="16">
         <f>F58-E58</f>
@@ -1945,10 +1945,10 @@
       <c r="C59" s="13" t="n"/>
       <c r="D59" s="38" t="n"/>
       <c r="E59" s="60" t="n">
-        <v>0.5805555555555556</v>
+        <v>0.5819444444444445</v>
       </c>
       <c r="F59" s="60" t="n">
-        <v>0.7604166666666666</v>
+        <v>0.7506944444444444</v>
       </c>
       <c r="G59" s="21">
         <f>F59-E59</f>
@@ -1970,10 +1970,10 @@
       <c r="C60" s="26" t="n"/>
       <c r="D60" s="37" t="n"/>
       <c r="E60" s="59" t="n">
-        <v>0.33125</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="F60" s="59" t="n">
-        <v>0.5034722222222222</v>
+        <v>0.4972222222222222</v>
       </c>
       <c r="G60" s="16">
         <f>F60-E60</f>
@@ -1990,10 +1990,10 @@
       <c r="C61" s="13" t="n"/>
       <c r="D61" s="38" t="n"/>
       <c r="E61" s="60" t="n">
-        <v>0.5895833333333333</v>
+        <v>0.5819444444444445</v>
       </c>
       <c r="F61" s="60" t="n">
-        <v>0.7569444444444444</v>
+        <v>0.7576388888888889</v>
       </c>
       <c r="G61" s="21">
         <f>F61-E61</f>
@@ -2019,10 +2019,10 @@
       <c r="C62" s="23" t="n"/>
       <c r="D62" s="23" t="n"/>
       <c r="E62" s="61" t="n">
-        <v>0.3354166666666666</v>
+        <v>0.33125</v>
       </c>
       <c r="F62" s="61" t="n">
-        <v>0.4972222222222222</v>
+        <v>0.4965277777777778</v>
       </c>
       <c r="G62" s="19" t="n"/>
       <c r="H62" s="34" t="n"/>

</xml_diff>